<commit_message>
introduced time variant covariates
</commit_message>
<xml_diff>
--- a/example_dat.xlsx
+++ b/example_dat.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="10">
   <si>
     <t xml:space="preserve">DATE</t>
   </si>
@@ -38,6 +38,15 @@
   </si>
   <si>
     <t xml:space="preserve">DUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIAL</t>
   </si>
   <si>
     <t xml:space="preserve">.</t>
@@ -148,10 +157,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -179,6 +188,15 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -191,13 +209,22 @@
         <v>1000</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>60</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -211,13 +238,22 @@
         <v>1000</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>60</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -227,17 +263,26 @@
       <c r="B4" s="2" t="n">
         <v>0.3</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>1000</v>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>60</v>
+        <v>2</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -245,19 +290,28 @@
         <v>43809</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0.581944444444444</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>16</v>
+        <v>0.3</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -265,70 +319,214 @@
         <v>43809</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.794444444444444</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>6</v>
+        <v>0.581944444444444</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>16</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>43810</v>
+        <v>43809</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.2875</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>1000</v>
+        <v>0.581944444444444</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>60</v>
+        <v>2</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
+        <v>43809</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>0.794444444444444</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
         <v>43810</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B9" s="2" t="n">
+        <v>0.2875</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>43810</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0.2875</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>43810</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>0.71875</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>43810</v>
+      </c>
+      <c r="B12" s="2" t="n">
         <v>0.760416666666667</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="0" t="n">
+      <c r="C12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="F12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
implemented and debugged time variable covariates
</commit_message>
<xml_diff>
--- a/example_dat.xlsx
+++ b/example_dat.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="10">
   <si>
     <t xml:space="preserve">DATE</t>
   </si>
@@ -157,10 +157,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -263,23 +263,23 @@
       <c r="B4" s="2" t="n">
         <v>0.3</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>9</v>
+      <c r="C4" s="0" t="n">
+        <v>1000</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>60</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="0" t="n">
-        <v>75</v>
+      <c r="H4" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>9</v>
@@ -290,19 +290,19 @@
         <v>43809</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>9</v>
+        <v>0.581944444444444</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>16</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>9</v>
@@ -319,19 +319,19 @@
         <v>43809</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.581944444444444</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>16</v>
+        <v>0.794444444444444</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>60</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>9</v>
@@ -345,25 +345,25 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>43809</v>
+        <v>43810</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.581944444444444</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>9</v>
+        <v>0.2875</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1000</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>75</v>
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>9</v>
@@ -374,22 +374,22 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>43809</v>
+        <v>43810</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.794444444444444</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>9</v>
+        <v>0.760416666666667</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>11</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>9</v>
@@ -401,132 +401,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>43810</v>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>0.2875</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>43810</v>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>0.2875</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>43810</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>0.71875</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
-        <v>43810</v>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>0.760416666666667</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>